<commit_message>
added missing survival data
</commit_message>
<xml_diff>
--- a/data/survival/Westcott/B_survival_09122024.xlsx
+++ b/data/survival/Westcott/B_survival_09122024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graceleuchtenberger/Library/Mobile Documents/com~apple~CloudDocs/Documents/project-gigas-conditioning-GL/data/survival/Westcott/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3FBF45F-DCF3-4347-ACD8-63E2B4579F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13513F35-F757-B54B-84C3-905894D5BA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3240" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{CA941532-24D2-184F-8B30-D5633C401736}"/>
   </bookViews>
@@ -529,7 +529,7 @@
   <dimension ref="A1:K121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="J118" sqref="J118"/>
+      <selection activeCell="I116" sqref="I116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4374,6 +4374,12 @@
       </c>
       <c r="H118">
         <v>7</v>
+      </c>
+      <c r="I118">
+        <v>50</v>
+      </c>
+      <c r="J118">
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>